<commit_message>
load+save tower location condition & wilayah, add fields for project information
</commit_message>
<xml_diff>
--- a/templates/input/tower_template.xlsx
+++ b/templates/input/tower_template.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Asumsi</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Ddr4</t>
   </si>
   <si>
-    <t>93A</t>
-  </si>
-  <si>
     <t>besar</t>
   </si>
   <si>
@@ -120,13 +117,34 @@
     <t>EARTH WIRE</t>
   </si>
   <si>
-    <t>Gelangan</t>
-  </si>
-  <si>
-    <t>ABCD</t>
-  </si>
-  <si>
     <t>Tarikan konduktor</t>
+  </si>
+  <si>
+    <t>Panjang haspel</t>
+  </si>
+  <si>
+    <t>Cibubur-Gandul</t>
+  </si>
+  <si>
+    <t>Unit Pelaksana</t>
+  </si>
+  <si>
+    <t>ACSR 2 Cct 1 X HAWK 240mm2</t>
+  </si>
+  <si>
+    <t>Perusahaan Pelaksana</t>
+  </si>
+  <si>
+    <t>Unit Induk</t>
+  </si>
+  <si>
+    <t>UNIT INDUK PEMBANGUNAN</t>
+  </si>
+  <si>
+    <t>JARINGAN JAWA BAGIAN TENGAH II</t>
+  </si>
+  <si>
+    <t>PT. FAST TRACK PROJECT</t>
   </si>
 </sst>
 </file>
@@ -192,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -606,14 +624,51 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="medium">
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -622,7 +677,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -637,16 +692,168 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -657,33 +864,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -691,137 +871,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1139,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M24"/>
+  <dimension ref="B2:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22:K23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,7 +1199,7 @@
     <col min="2" max="2" width="8.88671875" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="10.5546875" customWidth="1"/>
     <col min="12" max="12" width="11.33203125" customWidth="1"/>
@@ -1159,318 +1208,339 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="5">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="13"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="5">
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="9"/>
+        <v>27</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="14"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="5">
         <v>8</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="5">
         <v>1578</v>
       </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C7" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="55"/>
+      <c r="C7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="5">
         <v>13910</v>
       </c>
+      <c r="I7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="C9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="5">
+        <v>3600</v>
+      </c>
     </row>
     <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="32" t="s">
+      <c r="F14" s="29"/>
+      <c r="G14" s="15" t="s">
         <v>10</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="48" t="s">
+      <c r="I14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="32" t="s">
+      <c r="J14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="35" t="s">
+      <c r="K14" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="36"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="33"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C15" s="42"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="33"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="49"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33" t="s">
+      <c r="I15" s="18"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="33" t="s">
+      <c r="L15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="37" t="s">
+      <c r="M15" s="34" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="43"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="39" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="40"/>
+      <c r="F16" s="23"/>
       <c r="G16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="50"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="38"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="35"/>
     </row>
     <row r="17" spans="3:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="67"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
     </row>
     <row r="18" spans="3:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="29"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="19">
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="38">
         <v>60</v>
       </c>
-      <c r="H18" s="70"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="58"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C19" s="15">
+      <c r="C19" s="42">
         <v>1</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="44">
         <v>1</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="64">
         <v>0</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="23">
+      <c r="G19" s="39"/>
+      <c r="H19" s="66">
         <v>419</v>
       </c>
-      <c r="I19" s="54"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="58"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C20" s="16"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="7">
+      <c r="C20" s="43"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="38">
         <v>118.68</v>
       </c>
-      <c r="H20" s="24"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="58"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C21" s="15">
-        <v>104</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="12">
-        <v>0</v>
-      </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="23">
-        <v>420</v>
-      </c>
-      <c r="I21" s="54"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="58"/>
-    </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C22" s="16"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="19">
-        <v>225.04</v>
-      </c>
-      <c r="H22" s="24"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="58"/>
-    </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C23" s="59" t="s">
+      <c r="C21" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="58"/>
-    </row>
-    <row r="24" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="60"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="69"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
+    </row>
+    <row r="22" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="57"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="61"/>
+      <c r="M22" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I14:I16"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
@@ -1479,47 +1549,19 @@
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="I18:I19"/>
     <mergeCell ref="C7:E7"/>
-    <mergeCell ref="M18:M19"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="H19:H20"/>
-    <mergeCell ref="J20:J21"/>
     <mergeCell ref="G18:G19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="E16:F16"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="D14:D16"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="C21:F22"/>
+    <mergeCell ref="C9:E9"/>
     <mergeCell ref="C17:F18"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="C23:F24"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
     <mergeCell ref="H21:H22"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="F21:F22"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8">

</xml_diff>

<commit_message>
finale commit before UAT
</commit_message>
<xml_diff>
--- a/templates/input/tower_template.xlsx
+++ b/templates/input/tower_template.xlsx
@@ -698,102 +698,99 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -805,54 +802,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -871,6 +820,57 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1190,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1210,61 +1210,61 @@
       <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
       <c r="F3" s="5">
         <v>2</v>
       </c>
       <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="14"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="20"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
       <c r="F4" s="5">
         <v>4</v>
       </c>
       <c r="I4" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="14"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="20"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
       <c r="F5" s="5">
         <v>8</v>
       </c>
@@ -1282,270 +1282,237 @@
       <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="5">
         <v>1578</v>
       </c>
       <c r="I6" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="40"/>
       <c r="F7" s="5">
         <v>13910</v>
       </c>
       <c r="I7" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
       <c r="F8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I8" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="5">
         <v>3600</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="15" t="s">
+      <c r="F14" s="32"/>
+      <c r="G14" s="30" t="s">
         <v>10</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="J14" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="32" t="s">
+      <c r="K14" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="32"/>
-      <c r="M14" s="33"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="23"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C15" s="25"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="16"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16" t="s">
+      <c r="I15" s="36"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="16" t="s">
+      <c r="L15" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="34" t="s">
+      <c r="M15" s="26" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="22" t="s">
+      <c r="C16" s="55"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="23"/>
+      <c r="F16" s="29"/>
       <c r="G16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="19"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="35"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="27"/>
     </row>
     <row r="17" spans="3:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="48"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="64"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="36"/>
+      <c r="H17" s="12"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
     </row>
     <row r="18" spans="3:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="38">
+      <c r="C18" s="65"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="51">
         <v>60</v>
       </c>
-      <c r="H18" s="37"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C19" s="42">
+      <c r="C19" s="41">
         <v>1</v>
       </c>
-      <c r="D19" s="44">
+      <c r="D19" s="43">
         <v>1</v>
       </c>
-      <c r="E19" s="62" t="s">
+      <c r="E19" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="64">
+      <c r="F19" s="47">
         <v>0</v>
       </c>
-      <c r="G19" s="39"/>
-      <c r="H19" s="66">
+      <c r="G19" s="52"/>
+      <c r="H19" s="49">
         <v>419</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C20" s="43"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="38">
+      <c r="C20" s="42"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="51">
         <v>118.68</v>
       </c>
-      <c r="H20" s="67"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="60"/>
-      <c r="M21" s="60"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
     </row>
     <row r="22" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="57"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="61"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="61"/>
+      <c r="H22" s="15"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="61"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="I18:I19"/>
     <mergeCell ref="C7:E7"/>
@@ -1562,6 +1529,39 @@
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C17:F18"/>
     <mergeCell ref="H21:H22"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="L19:L20"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8">

</xml_diff>